<commit_message>
script para apagar pastas vetores e positivas
</commit_message>
<xml_diff>
--- a/Casos.xlsx
+++ b/Casos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\POC-TCC-CLASSIFIER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A9FF15-A45C-4C86-B3C2-ABB83745AB6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6BBB72-C891-49FA-88F3-20B0BDD6AE15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos" sheetId="5" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5184" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5186" uniqueCount="116">
   <si>
     <t>N Caso</t>
   </si>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE338563-A398-4B7E-9DA2-C2EF8ABE1454}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33430,8 +33430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D272F9-C60B-4199-8657-134ADD5033E3}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33530,6 +33530,9 @@
       <c r="B7" t="s">
         <v>113</v>
       </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
       <c r="I7">
         <v>5</v>
       </c>
@@ -33543,6 +33546,9 @@
       </c>
       <c r="B8" t="s">
         <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
treinamento - versao 6 do classificador
</commit_message>
<xml_diff>
--- a/Casos.xlsx
+++ b/Casos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\POC-TCC-CLASSIFIER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6BBB72-C891-49FA-88F3-20B0BDD6AE15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9411321-F075-4B46-A86A-0525C3213DA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos" sheetId="5" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5186" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5187" uniqueCount="116">
   <si>
     <t>N Caso</t>
   </si>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE338563-A398-4B7E-9DA2-C2EF8ABE1454}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,6 +1114,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
       <c r="B7">
         <v>6</v>
       </c>
@@ -33430,7 +33433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D272F9-C60B-4199-8657-134ADD5033E3}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
treinamento - versao 7
</commit_message>
<xml_diff>
--- a/Casos.xlsx
+++ b/Casos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\POC-TCC-CLASSIFIER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9411321-F075-4B46-A86A-0525C3213DA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897222D9-27DF-4CED-A58E-E226E2273E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5187" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5188" uniqueCount="116">
   <si>
     <t>N Caso</t>
   </si>
@@ -842,7 +842,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,6 +1156,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
       <c r="B8">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
treinamento - versao 17
</commit_message>
<xml_diff>
--- a/Casos.xlsx
+++ b/Casos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\POC-TCC-CLASSIFIER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C01ACC-1D19-4D55-9E64-A8D5BE33B521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AC26ED-CE7F-4F22-8C86-1CACD9930399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27630" yWindow="3330" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="3" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos" sheetId="5" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5202" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5204" uniqueCount="122">
   <si>
     <t>N Caso</t>
   </si>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE338563-A398-4B7E-9DA2-C2EF8ABE1454}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,6 +1536,9 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
       <c r="B16">
         <v>15</v>
       </c>
@@ -1574,7 +1577,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
       <c r="B17">
         <v>16</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>17</v>
       </c>
@@ -1652,7 +1658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>18</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>19</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>20</v>
       </c>
@@ -1769,7 +1775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>21</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
@@ -1847,7 +1853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>25</v>
       </c>
@@ -1964,7 +1970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>26</v>
       </c>
@@ -2003,7 +2009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>28</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>29</v>
       </c>
@@ -2120,7 +2126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>30</v>
       </c>
@@ -33642,7 +33648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77CCE48-7B7D-463E-97D6-7C4A5240B20A}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
treinamento - versao 19
</commit_message>
<xml_diff>
--- a/Casos.xlsx
+++ b/Casos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\POC-TCC-CLASSIFIER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AC26ED-CE7F-4F22-8C86-1CACD9930399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BA9C9-BF91-4BBA-9DC9-518DAB7D3628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5204" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5269" uniqueCount="126">
   <si>
     <t>N Caso</t>
   </si>
@@ -464,12 +464,24 @@
   <si>
     <t>False-Negative Rate = FN / FN + TP</t>
   </si>
+  <si>
+    <t>featureType</t>
+  </si>
+  <si>
+    <t>HAAR(default)</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>BASIC (default)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,6 +531,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -553,7 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -568,6 +593,8 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -883,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE338563-A398-4B7E-9DA2-C2EF8ABE1454}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,10 +927,11 @@
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -943,11 +971,17 @@
       <c r="M1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -955,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f>CONCATENATE("V-",B2,"-",D2,"-",E2,"-",G2,"-",K2,"-",L2,"-",N2)</f>
+        <f>CONCATENATE("V-",B2,"-",D2,"-",E2,"-",G2,"-",K2,"-",L2,"-",P2)</f>
         <v>V-1-1-800-2-10-GS-</v>
       </c>
       <c r="D2">
@@ -988,8 +1022,14 @@
       <c r="M2">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N2" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -997,7 +1037,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C31" si="0">CONCATENATE("V-",B3,"-",D3,"-",E3,"-",G3,"-",K3,"-",L3,"-",N3)</f>
+        <f>CONCATENATE("V-",B3,"-",D3,"-",E3,"-",G3,"-",K3,"-",L3,"-",P3)</f>
         <v>V-2-2-800-2-10-GS-</v>
       </c>
       <c r="D3">
@@ -1007,18 +1047,18 @@
         <v>800</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F31" si="1">E3*G3</f>
+        <f t="shared" ref="F3:F31" si="0">E3*G3</f>
         <v>1600</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="2">F3*1.125</f>
+        <f t="shared" ref="I3:I7" si="1">F3*1.125</f>
         <v>1800</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J7" si="3">I3/D3</f>
+        <f t="shared" ref="J3:J7" si="2">I3/D3</f>
         <v>900</v>
       </c>
       <c r="K3">
@@ -1030,8 +1070,14 @@
       <c r="M3">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N3" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1039,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B4,"-",D4,"-",E4,"-",G4,"-",K4,"-",L4,"-",P4)</f>
         <v>V-3-5-800-2-10-GS-</v>
       </c>
       <c r="D4">
@@ -1049,18 +1095,18 @@
         <v>800</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="I4">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="2"/>
-        <v>1800</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="3"/>
         <v>360</v>
       </c>
       <c r="K4">
@@ -1072,8 +1118,14 @@
       <c r="M4">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -1081,7 +1133,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B5,"-",D5,"-",E5,"-",G5,"-",K5,"-",L5,"-",P5)</f>
         <v>V-4-10-800-2-10-GS-</v>
       </c>
       <c r="D5">
@@ -1091,18 +1143,18 @@
         <v>800</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="2"/>
-        <v>1800</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="K5">
@@ -1114,8 +1166,14 @@
       <c r="M5">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -1123,7 +1181,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B6,"-",D6,"-",E6,"-",G6,"-",K6,"-",L6,"-",P6)</f>
         <v>V-5-25-800-2-10-GS-</v>
       </c>
       <c r="D6">
@@ -1133,18 +1191,18 @@
         <v>800</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="I6">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="2"/>
-        <v>1800</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="K6">
@@ -1156,8 +1214,14 @@
       <c r="M6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -1165,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B7,"-",D7,"-",E7,"-",G7,"-",K7,"-",L7,"-",P7)</f>
         <v>V-6-50-800-2-10-GS-</v>
       </c>
       <c r="D7">
@@ -1175,18 +1239,18 @@
         <v>800</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="I7">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="2"/>
-        <v>1800</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="K7">
@@ -1198,8 +1262,14 @@
       <c r="M7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -1207,7 +1277,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B8,"-",D8,"-",E8,"-",G8,"-",K8,"-",L8,"-",P8)</f>
         <v>V-7-1-1000-2-10-GS-</v>
       </c>
       <c r="D8">
@@ -1217,18 +1287,18 @@
         <v>1000</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I25" si="4">F8*1.125</f>
+        <f t="shared" ref="I8:I25" si="3">F8*1.125</f>
         <v>2250</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J25" si="5">I8/D8</f>
+        <f t="shared" ref="J8:J25" si="4">I8/D8</f>
         <v>2250</v>
       </c>
       <c r="K8">
@@ -1240,8 +1310,14 @@
       <c r="M8">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -1249,7 +1325,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B9,"-",D9,"-",E9,"-",G9,"-",K9,"-",L9,"-",P9)</f>
         <v>V-8-2-1000-2-10-GS-</v>
       </c>
       <c r="D9">
@@ -1259,551 +1335,638 @@
         <v>1000</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="I9">
+        <f t="shared" si="3"/>
+        <v>2250</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>1125</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+      <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9">
+        <v>18</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="str">
+        <f>CONCATENATE("V-",B10,"-",D10,"-",E10,"-",G10,"-",K10,"-",L10,"-",P10)</f>
+        <v>V-9-5-1000-2-10-GS-</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1000</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>2250</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>450</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10">
+        <v>18</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <f>CONCATENATE("V-",B11,"-",D11,"-",E11,"-",G11,"-",K11,"-",L11,"-",P11)</f>
+        <v>V-10-10-1000-2-10-GS-</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1000</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>2250</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>225</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M11">
+        <v>18</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <f>CONCATENATE("V-",B12,"-",D12,"-",E12,"-",G12,"-",K12,"-",L12,"-",P12)</f>
+        <v>V-11-25-1000-2-10-GS-</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>1000</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>2250</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12">
+        <v>18</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="str">
+        <f>CONCATENATE("V-",B13,"-",D13,"-",E13,"-",G13,"-",K13,"-",L13,"-",P13)</f>
+        <v>V-12-50-1000-2-10-GS-</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>1000</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>2250</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13">
+        <v>18</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE("V-",B14,"-",D14,"-",E14,"-",G14,"-",K14,"-",L14,"-",P14)</f>
+        <v>V-13-1-2500-2-10-GS-</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2500</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>5625</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>5625</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14">
+        <v>18</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>CONCATENATE("V-",B15,"-",D15,"-",E15,"-",G15,"-",K15,"-",L15,"-",P15)</f>
+        <v>V-14-2-2500-2-10-GS-</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2500</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>5625</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>2812.5</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M15">
+        <v>18</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="str">
+        <f>CONCATENATE("V-",B16,"-",D16,"-",E16,"-",G16,"-",K16,"-",L16,"-",P16)</f>
+        <v>V-15-5-2500-2-10-GS-</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>2500</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>5625</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>1125</v>
+      </c>
+      <c r="K16">
+        <v>10</v>
+      </c>
+      <c r="L16" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16">
+        <v>18</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="str">
+        <f>CONCATENATE("V-",B17,"-",D17,"-",E17,"-",G17,"-",K17,"-",L17,"-",P17)</f>
+        <v>V-16-10-2500-2-10-GS-</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <v>2500</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>5625</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>562.5</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="L17" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17">
+        <v>18</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="str">
+        <f>CONCATENATE("V-",B18,"-",D18,"-",E18,"-",G18,"-",K18,"-",L18,"-",P18)</f>
+        <v>V-17-25-2500-2-10-GS-</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+      <c r="E18">
+        <v>2500</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>5625</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="4"/>
+        <v>225</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18">
+        <v>18</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="str">
+        <f>CONCATENATE("V-",B19,"-",D19,"-",E19,"-",G19,"-",K19,"-",L19,"-",P19)</f>
+        <v>V-18-50-2500-2-10-GS-</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <v>2500</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>5625</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="4"/>
+        <v>112.5</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19">
+        <v>18</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="str">
+        <f>CONCATENATE("V-",B20,"-",D20,"-",E20,"-",G20,"-",K20,"-",L20,"-",P20)</f>
+        <v>V-19-1-5000-2-10-GS-</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>5000</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>11250</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="4"/>
+        <v>11250</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20">
+        <v>18</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="str">
+        <f>CONCATENATE("V-",B21,"-",D21,"-",E21,"-",G21,"-",K21,"-",L21,"-",P21)</f>
+        <v>V-20-2-5000-2-10-GS-</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>5000</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>11250</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="4"/>
+        <v>5625</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21" t="s">
+        <v>66</v>
+      </c>
+      <c r="M21">
+        <v>18</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O21" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="str">
+        <f>CONCATENATE("V-",B22,"-",D22,"-",E22,"-",G22,"-",K22,"-",L22,"-",P22)</f>
+        <v>V-21-5-5000-2-10-GS-</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>5000</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>11250</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="4"/>
         <v>2250</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="5"/>
-        <v>1125</v>
-      </c>
-      <c r="K9">
-        <v>10</v>
-      </c>
-      <c r="L9" t="s">
-        <v>66</v>
-      </c>
-      <c r="M9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>V-9-5-1000-2-10-GS-</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>1000</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>2000</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="4"/>
-        <v>2250</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="5"/>
-        <v>450</v>
-      </c>
-      <c r="K10">
-        <v>10</v>
-      </c>
-      <c r="L10" t="s">
-        <v>66</v>
-      </c>
-      <c r="M10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>V-10-10-1000-2-10-GS-</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>1000</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>2000</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="4"/>
-        <v>2250</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="5"/>
-        <v>225</v>
-      </c>
-      <c r="K11">
-        <v>10</v>
-      </c>
-      <c r="L11" t="s">
-        <v>66</v>
-      </c>
-      <c r="M11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>V-11-25-1000-2-10-GS-</v>
-      </c>
-      <c r="D12">
-        <v>25</v>
-      </c>
-      <c r="E12">
-        <v>1000</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>2000</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="4"/>
-        <v>2250</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="5"/>
-        <v>90</v>
-      </c>
-      <c r="K12">
-        <v>10</v>
-      </c>
-      <c r="L12" t="s">
-        <v>66</v>
-      </c>
-      <c r="M12">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>V-12-50-1000-2-10-GS-</v>
-      </c>
-      <c r="D13">
-        <v>50</v>
-      </c>
-      <c r="E13">
-        <v>1000</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>2000</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="4"/>
-        <v>2250</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>45</v>
-      </c>
-      <c r="K13">
-        <v>10</v>
-      </c>
-      <c r="L13" t="s">
-        <v>66</v>
-      </c>
-      <c r="M13">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>V-13-1-2500-2-10-GS-</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>2500</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="4"/>
-        <v>5625</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
-        <v>5625</v>
-      </c>
-      <c r="K14">
-        <v>10</v>
-      </c>
-      <c r="L14" t="s">
-        <v>66</v>
-      </c>
-      <c r="M14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>V-14-2-2500-2-10-GS-</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>2500</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="4"/>
-        <v>5625</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="5"/>
-        <v>2812.5</v>
-      </c>
-      <c r="K15">
-        <v>10</v>
-      </c>
-      <c r="L15" t="s">
-        <v>66</v>
-      </c>
-      <c r="M15">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>V-15-5-2500-2-10-GS-</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>2500</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="4"/>
-        <v>5625</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="5"/>
-        <v>1125</v>
-      </c>
-      <c r="K16">
-        <v>10</v>
-      </c>
-      <c r="L16" t="s">
-        <v>66</v>
-      </c>
-      <c r="M16">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>V-16-10-2500-2-10-GS-</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="E17">
-        <v>2500</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="4"/>
-        <v>5625</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="5"/>
-        <v>562.5</v>
-      </c>
-      <c r="K17">
-        <v>10</v>
-      </c>
-      <c r="L17" t="s">
-        <v>66</v>
-      </c>
-      <c r="M17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>V-17-25-2500-2-10-GS-</v>
-      </c>
-      <c r="D18">
-        <v>25</v>
-      </c>
-      <c r="E18">
-        <v>2500</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="4"/>
-        <v>5625</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="5"/>
-        <v>225</v>
-      </c>
-      <c r="K18">
-        <v>10</v>
-      </c>
-      <c r="L18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>V-18-50-2500-2-10-GS-</v>
-      </c>
-      <c r="D19">
-        <v>50</v>
-      </c>
-      <c r="E19">
-        <v>2500</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="4"/>
-        <v>5625</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
-        <v>112.5</v>
-      </c>
-      <c r="K19">
-        <v>10</v>
-      </c>
-      <c r="L19" t="s">
-        <v>66</v>
-      </c>
-      <c r="M19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>V-19-1-5000-2-10-GS-</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>5000</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>10000</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="4"/>
-        <v>11250</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="5"/>
-        <v>11250</v>
-      </c>
-      <c r="K20">
-        <v>10</v>
-      </c>
-      <c r="L20" t="s">
-        <v>66</v>
-      </c>
-      <c r="M20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>V-20-2-5000-2-10-GS-</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <v>5000</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>10000</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="4"/>
-        <v>11250</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="5"/>
-        <v>5625</v>
-      </c>
-      <c r="K21">
-        <v>10</v>
-      </c>
-      <c r="L21" t="s">
-        <v>66</v>
-      </c>
-      <c r="M21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>V-21-5-5000-2-10-GS-</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <v>5000</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
-        <v>10000</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="4"/>
-        <v>11250</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="5"/>
-        <v>2250</v>
-      </c>
       <c r="K22">
         <v>10</v>
       </c>
@@ -1813,13 +1976,19 @@
       <c r="M22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B23,"-",D23,"-",E23,"-",G23,"-",K23,"-",L23,"-",P23)</f>
         <v>V-22-10-5000-2-10-GS-</v>
       </c>
       <c r="D23">
@@ -1829,18 +1998,18 @@
         <v>5000</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="I23">
+        <f t="shared" si="3"/>
+        <v>11250</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="4"/>
-        <v>11250</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="5"/>
         <v>1125</v>
       </c>
       <c r="K23">
@@ -1852,13 +2021,19 @@
       <c r="M23">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B24,"-",D24,"-",E24,"-",G24,"-",K24,"-",L24,"-",P24)</f>
         <v>V-23-25-5000-2-10-GS-</v>
       </c>
       <c r="D24">
@@ -1868,18 +2043,18 @@
         <v>5000</v>
       </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="I24">
+        <f t="shared" si="3"/>
+        <v>11250</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="4"/>
-        <v>11250</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="5"/>
         <v>450</v>
       </c>
       <c r="K24">
@@ -1891,13 +2066,19 @@
       <c r="M24">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O24" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B25,"-",D25,"-",E25,"-",G25,"-",K25,"-",L25,"-",P25)</f>
         <v>V-24-50-5000-2-10-GS-</v>
       </c>
       <c r="D25">
@@ -1907,18 +2088,18 @@
         <v>5000</v>
       </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="I25">
+        <f t="shared" si="3"/>
+        <v>11250</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="4"/>
-        <v>11250</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="5"/>
         <v>225</v>
       </c>
       <c r="K25">
@@ -1930,13 +2111,19 @@
       <c r="M25">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O25" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B26,"-",D26,"-",E26,"-",G26,"-",K26,"-",L26,"-",P26)</f>
         <v>V-25-1-10000-2-10-GS-</v>
       </c>
       <c r="D26">
@@ -1946,18 +2133,18 @@
         <v>10000</v>
       </c>
       <c r="F26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I26:I31" si="6">F26*1.125</f>
+        <f t="shared" ref="I26:I31" si="5">F26*1.125</f>
         <v>22500</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J31" si="7">I26/D26</f>
+        <f t="shared" ref="J26:J31" si="6">I26/D26</f>
         <v>22500</v>
       </c>
       <c r="K26">
@@ -1969,13 +2156,19 @@
       <c r="M26">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O26" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B27,"-",D27,"-",E27,"-",G27,"-",K27,"-",L27,"-",P27)</f>
         <v>V-26-2-10000-2-10-GS-</v>
       </c>
       <c r="D27">
@@ -1985,18 +2178,18 @@
         <v>10000</v>
       </c>
       <c r="F27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
       <c r="I27">
+        <f t="shared" si="5"/>
+        <v>22500</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="6"/>
-        <v>22500</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="7"/>
         <v>11250</v>
       </c>
       <c r="K27">
@@ -2008,13 +2201,19 @@
       <c r="M27">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O27" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B28,"-",D28,"-",E28,"-",G28,"-",K28,"-",L28,"-",P28)</f>
         <v>V-27-5-10000-2-10-GS-</v>
       </c>
       <c r="D28">
@@ -2024,18 +2223,18 @@
         <v>10000</v>
       </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="G28">
         <v>2</v>
       </c>
       <c r="I28">
+        <f t="shared" si="5"/>
+        <v>22500</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="6"/>
-        <v>22500</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="7"/>
         <v>4500</v>
       </c>
       <c r="K28">
@@ -2047,13 +2246,19 @@
       <c r="M28">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O28" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B29,"-",D29,"-",E29,"-",G29,"-",K29,"-",L29,"-",P29)</f>
         <v>V-28-10-10000-2-10-GS-</v>
       </c>
       <c r="D29">
@@ -2063,18 +2268,18 @@
         <v>10000</v>
       </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="G29">
         <v>2</v>
       </c>
       <c r="I29">
+        <f t="shared" si="5"/>
+        <v>22500</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="6"/>
-        <v>22500</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="7"/>
         <v>2250</v>
       </c>
       <c r="K29">
@@ -2086,13 +2291,19 @@
       <c r="M29">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O29" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B30,"-",D30,"-",E30,"-",G30,"-",K30,"-",L30,"-",P30)</f>
         <v>V-29-25-10000-2-10-GS-</v>
       </c>
       <c r="D30">
@@ -2102,18 +2313,18 @@
         <v>10000</v>
       </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="I30">
+        <f t="shared" si="5"/>
+        <v>22500</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="6"/>
-        <v>22500</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="7"/>
         <v>900</v>
       </c>
       <c r="K30">
@@ -2125,13 +2336,19 @@
       <c r="M30">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("V-",B31,"-",D31,"-",E31,"-",G31,"-",K31,"-",L31,"-",P31)</f>
         <v>V-30-50-10000-2-10-GS-</v>
       </c>
       <c r="D31">
@@ -2141,18 +2358,18 @@
         <v>10000</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20000</v>
       </c>
       <c r="G31">
         <v>2</v>
       </c>
       <c r="I31">
+        <f t="shared" si="5"/>
+        <v>22500</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="6"/>
-        <v>22500</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="7"/>
         <v>450</v>
       </c>
       <c r="K31">
@@ -2163,6 +2380,12 @@
       </c>
       <c r="M31">
         <v>18</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
treinamento - versao 20
</commit_message>
<xml_diff>
--- a/Casos.xlsx
+++ b/Casos.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\POC-TCC-CLASSIFIER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BA9C9-BF91-4BBA-9DC9-518DAB7D3628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFD110F-DE3A-484A-99C1-DEDEB7348191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{C01B60D5-4781-4C39-AB84-F2896830E0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos" sheetId="5" r:id="rId1"/>
-    <sheet name="Parametros Classificador" sheetId="7" r:id="rId2"/>
-    <sheet name="TODO" sheetId="4" r:id="rId3"/>
-    <sheet name="Calculo de Precisao" sheetId="6" r:id="rId4"/>
-    <sheet name="Resultados" sheetId="2" r:id="rId5"/>
-    <sheet name="RASCUNHO QUERO" sheetId="3" r:id="rId6"/>
+    <sheet name="quantidade de casos" sheetId="9" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="8" r:id="rId3"/>
+    <sheet name="Parametros Classificador" sheetId="7" r:id="rId4"/>
+    <sheet name="TODO" sheetId="4" r:id="rId5"/>
+    <sheet name="Calculo de Precisao" sheetId="6" r:id="rId6"/>
+    <sheet name="Resultados" sheetId="2" r:id="rId7"/>
+    <sheet name="RASCUNHO QUERO" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -97,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5269" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5289" uniqueCount="145">
   <si>
     <t>N Caso</t>
   </si>
@@ -475,6 +477,63 @@
   </si>
   <si>
     <t>BASIC (default)</t>
+  </si>
+  <si>
+    <t>Negativos</t>
+  </si>
+  <si>
+    <t>Numero Rotacionado</t>
+  </si>
+  <si>
+    <t>Total negativos</t>
+  </si>
+  <si>
+    <t>FeatureType</t>
+  </si>
+  <si>
+    <t>N de Numero de casos</t>
+  </si>
+  <si>
+    <t>18,19,20</t>
+  </si>
+  <si>
+    <t>8,9,10,11,12,13,14,15</t>
+  </si>
+  <si>
+    <t>filtros</t>
+  </si>
+  <si>
+    <t>GS,?,?</t>
+  </si>
+  <si>
+    <t>proporção</t>
+  </si>
+  <si>
+    <t>0.25,0.5,1,2,10,100</t>
+  </si>
+  <si>
+    <t>Adicionar mais</t>
+  </si>
+  <si>
+    <t>negativos</t>
+  </si>
+  <si>
+    <t>n objetos</t>
+  </si>
+  <si>
+    <t>1,2,5,10,25,50,200</t>
+  </si>
+  <si>
+    <t>quantidade de opcoes</t>
+  </si>
+  <si>
+    <t>opcoes</t>
+  </si>
+  <si>
+    <t>Parametros de treinamento</t>
+  </si>
+  <si>
+    <t>TOTAL DE CASOS PARA CRIAR O CLASSIFICADOR</t>
   </si>
 </sst>
 </file>
@@ -912,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE338563-A398-4B7E-9DA2-C2EF8ABE1454}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f>CONCATENATE("V-",B2,"-",D2,"-",E2,"-",G2,"-",K2,"-",L2,"-",P2)</f>
+        <f t="shared" ref="C2:C31" si="0">CONCATENATE("V-",B2,"-",D2,"-",E2,"-",G2,"-",K2,"-",L2,"-",P2)</f>
         <v>V-1-1-800-2-10-GS-</v>
       </c>
       <c r="D2">
@@ -1037,7 +1096,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="str">
-        <f>CONCATENATE("V-",B3,"-",D3,"-",E3,"-",G3,"-",K3,"-",L3,"-",P3)</f>
+        <f t="shared" si="0"/>
         <v>V-2-2-800-2-10-GS-</v>
       </c>
       <c r="D3">
@@ -1047,18 +1106,18 @@
         <v>800</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F31" si="0">E3*G3</f>
+        <f t="shared" ref="F3:F31" si="1">E3*G3</f>
         <v>1600</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="1">F3*1.125</f>
+        <f t="shared" ref="I3:I7" si="2">F3*1.125</f>
         <v>1800</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J7" si="2">I3/D3</f>
+        <f t="shared" ref="J3:J7" si="3">I3/D3</f>
         <v>900</v>
       </c>
       <c r="K3">
@@ -1085,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="str">
-        <f>CONCATENATE("V-",B4,"-",D4,"-",E4,"-",G4,"-",K4,"-",L4,"-",P4)</f>
+        <f t="shared" si="0"/>
         <v>V-3-5-800-2-10-GS-</v>
       </c>
       <c r="D4">
@@ -1095,18 +1154,18 @@
         <v>800</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1600</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
       <c r="K4">
@@ -1133,7 +1192,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="str">
-        <f>CONCATENATE("V-",B5,"-",D5,"-",E5,"-",G5,"-",K5,"-",L5,"-",P5)</f>
+        <f t="shared" si="0"/>
         <v>V-4-10-800-2-10-GS-</v>
       </c>
       <c r="D5">
@@ -1143,18 +1202,18 @@
         <v>800</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1600</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="K5">
@@ -1181,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="str">
-        <f>CONCATENATE("V-",B6,"-",D6,"-",E6,"-",G6,"-",K6,"-",L6,"-",P6)</f>
+        <f t="shared" si="0"/>
         <v>V-5-25-800-2-10-GS-</v>
       </c>
       <c r="D6">
@@ -1191,18 +1250,18 @@
         <v>800</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1600</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="K6">
@@ -1229,7 +1288,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="str">
-        <f>CONCATENATE("V-",B7,"-",D7,"-",E7,"-",G7,"-",K7,"-",L7,"-",P7)</f>
+        <f t="shared" si="0"/>
         <v>V-6-50-800-2-10-GS-</v>
       </c>
       <c r="D7">
@@ -1239,18 +1298,18 @@
         <v>800</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1600</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="K7">
@@ -1277,7 +1336,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="str">
-        <f>CONCATENATE("V-",B8,"-",D8,"-",E8,"-",G8,"-",K8,"-",L8,"-",P8)</f>
+        <f t="shared" si="0"/>
         <v>V-7-1-1000-2-10-GS-</v>
       </c>
       <c r="D8">
@@ -1287,18 +1346,18 @@
         <v>1000</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I25" si="3">F8*1.125</f>
+        <f t="shared" ref="I8:I25" si="4">F8*1.125</f>
         <v>2250</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J25" si="4">I8/D8</f>
+        <f t="shared" ref="J8:J25" si="5">I8/D8</f>
         <v>2250</v>
       </c>
       <c r="K8">
@@ -1325,7 +1384,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="str">
-        <f>CONCATENATE("V-",B9,"-",D9,"-",E9,"-",G9,"-",K9,"-",L9,"-",P9)</f>
+        <f t="shared" si="0"/>
         <v>V-8-2-1000-2-10-GS-</v>
       </c>
       <c r="D9">
@@ -1335,18 +1394,18 @@
         <v>1000</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2250</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1125</v>
       </c>
       <c r="K9">
@@ -1373,7 +1432,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="str">
-        <f>CONCATENATE("V-",B10,"-",D10,"-",E10,"-",G10,"-",K10,"-",L10,"-",P10)</f>
+        <f t="shared" si="0"/>
         <v>V-9-5-1000-2-10-GS-</v>
       </c>
       <c r="D10">
@@ -1383,18 +1442,18 @@
         <v>1000</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="I10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2250</v>
       </c>
       <c r="J10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>450</v>
       </c>
       <c r="K10">
@@ -1421,7 +1480,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="str">
-        <f>CONCATENATE("V-",B11,"-",D11,"-",E11,"-",G11,"-",K11,"-",L11,"-",P11)</f>
+        <f t="shared" si="0"/>
         <v>V-10-10-1000-2-10-GS-</v>
       </c>
       <c r="D11">
@@ -1431,18 +1490,18 @@
         <v>1000</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2250</v>
       </c>
       <c r="J11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>225</v>
       </c>
       <c r="K11">
@@ -1469,7 +1528,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="str">
-        <f>CONCATENATE("V-",B12,"-",D12,"-",E12,"-",G12,"-",K12,"-",L12,"-",P12)</f>
+        <f t="shared" si="0"/>
         <v>V-11-25-1000-2-10-GS-</v>
       </c>
       <c r="D12">
@@ -1479,18 +1538,18 @@
         <v>1000</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2250</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="K12">
@@ -1517,7 +1576,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="str">
-        <f>CONCATENATE("V-",B13,"-",D13,"-",E13,"-",G13,"-",K13,"-",L13,"-",P13)</f>
+        <f t="shared" si="0"/>
         <v>V-12-50-1000-2-10-GS-</v>
       </c>
       <c r="D13">
@@ -1527,18 +1586,18 @@
         <v>1000</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="I13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2250</v>
       </c>
       <c r="J13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="K13">
@@ -1565,7 +1624,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="str">
-        <f>CONCATENATE("V-",B14,"-",D14,"-",E14,"-",G14,"-",K14,"-",L14,"-",P14)</f>
+        <f t="shared" si="0"/>
         <v>V-13-1-2500-2-10-GS-</v>
       </c>
       <c r="D14">
@@ -1575,18 +1634,18 @@
         <v>2500</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5625</v>
       </c>
       <c r="J14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5625</v>
       </c>
       <c r="K14">
@@ -1613,7 +1672,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="str">
-        <f>CONCATENATE("V-",B15,"-",D15,"-",E15,"-",G15,"-",K15,"-",L15,"-",P15)</f>
+        <f t="shared" si="0"/>
         <v>V-14-2-2500-2-10-GS-</v>
       </c>
       <c r="D15">
@@ -1623,18 +1682,18 @@
         <v>2500</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="I15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5625</v>
       </c>
       <c r="J15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2812.5</v>
       </c>
       <c r="K15">
@@ -1661,7 +1720,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="str">
-        <f>CONCATENATE("V-",B16,"-",D16,"-",E16,"-",G16,"-",K16,"-",L16,"-",P16)</f>
+        <f t="shared" si="0"/>
         <v>V-15-5-2500-2-10-GS-</v>
       </c>
       <c r="D16">
@@ -1671,18 +1730,18 @@
         <v>2500</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
       <c r="I16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5625</v>
       </c>
       <c r="J16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1125</v>
       </c>
       <c r="K16">
@@ -1709,7 +1768,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="str">
-        <f>CONCATENATE("V-",B17,"-",D17,"-",E17,"-",G17,"-",K17,"-",L17,"-",P17)</f>
+        <f t="shared" si="0"/>
         <v>V-16-10-2500-2-10-GS-</v>
       </c>
       <c r="D17">
@@ -1719,18 +1778,18 @@
         <v>2500</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="I17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5625</v>
       </c>
       <c r="J17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>562.5</v>
       </c>
       <c r="K17">
@@ -1757,7 +1816,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="str">
-        <f>CONCATENATE("V-",B18,"-",D18,"-",E18,"-",G18,"-",K18,"-",L18,"-",P18)</f>
+        <f t="shared" si="0"/>
         <v>V-17-25-2500-2-10-GS-</v>
       </c>
       <c r="D18">
@@ -1767,18 +1826,18 @@
         <v>2500</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="I18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5625</v>
       </c>
       <c r="J18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>225</v>
       </c>
       <c r="K18">
@@ -1805,7 +1864,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="str">
-        <f>CONCATENATE("V-",B19,"-",D19,"-",E19,"-",G19,"-",K19,"-",L19,"-",P19)</f>
+        <f t="shared" si="0"/>
         <v>V-18-50-2500-2-10-GS-</v>
       </c>
       <c r="D19">
@@ -1815,18 +1874,18 @@
         <v>2500</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5625</v>
       </c>
       <c r="J19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>112.5</v>
       </c>
       <c r="K19">
@@ -1853,7 +1912,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="str">
-        <f>CONCATENATE("V-",B20,"-",D20,"-",E20,"-",G20,"-",K20,"-",L20,"-",P20)</f>
+        <f t="shared" si="0"/>
         <v>V-19-1-5000-2-10-GS-</v>
       </c>
       <c r="D20">
@@ -1863,18 +1922,18 @@
         <v>5000</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="I20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11250</v>
       </c>
       <c r="J20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>11250</v>
       </c>
       <c r="K20">
@@ -1898,7 +1957,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="str">
-        <f>CONCATENATE("V-",B21,"-",D21,"-",E21,"-",G21,"-",K21,"-",L21,"-",P21)</f>
+        <f t="shared" si="0"/>
         <v>V-20-2-5000-2-10-GS-</v>
       </c>
       <c r="D21">
@@ -1908,18 +1967,18 @@
         <v>5000</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="I21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11250</v>
       </c>
       <c r="J21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5625</v>
       </c>
       <c r="K21">
@@ -1943,7 +2002,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="str">
-        <f>CONCATENATE("V-",B22,"-",D22,"-",E22,"-",G22,"-",K22,"-",L22,"-",P22)</f>
+        <f t="shared" si="0"/>
         <v>V-21-5-5000-2-10-GS-</v>
       </c>
       <c r="D22">
@@ -1953,18 +2012,18 @@
         <v>5000</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11250</v>
       </c>
       <c r="J22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2250</v>
       </c>
       <c r="K22">
@@ -1988,7 +2047,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="str">
-        <f>CONCATENATE("V-",B23,"-",D23,"-",E23,"-",G23,"-",K23,"-",L23,"-",P23)</f>
+        <f t="shared" si="0"/>
         <v>V-22-10-5000-2-10-GS-</v>
       </c>
       <c r="D23">
@@ -1998,18 +2057,18 @@
         <v>5000</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="I23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11250</v>
       </c>
       <c r="J23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1125</v>
       </c>
       <c r="K23">
@@ -2033,7 +2092,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="str">
-        <f>CONCATENATE("V-",B24,"-",D24,"-",E24,"-",G24,"-",K24,"-",L24,"-",P24)</f>
+        <f t="shared" si="0"/>
         <v>V-23-25-5000-2-10-GS-</v>
       </c>
       <c r="D24">
@@ -2043,18 +2102,18 @@
         <v>5000</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="I24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11250</v>
       </c>
       <c r="J24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>450</v>
       </c>
       <c r="K24">
@@ -2078,7 +2137,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="str">
-        <f>CONCATENATE("V-",B25,"-",D25,"-",E25,"-",G25,"-",K25,"-",L25,"-",P25)</f>
+        <f t="shared" si="0"/>
         <v>V-24-50-5000-2-10-GS-</v>
       </c>
       <c r="D25">
@@ -2088,18 +2147,18 @@
         <v>5000</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10000</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="I25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11250</v>
       </c>
       <c r="J25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>225</v>
       </c>
       <c r="K25">
@@ -2123,7 +2182,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="str">
-        <f>CONCATENATE("V-",B26,"-",D26,"-",E26,"-",G26,"-",K26,"-",L26,"-",P26)</f>
+        <f t="shared" si="0"/>
         <v>V-25-1-10000-2-10-GS-</v>
       </c>
       <c r="D26">
@@ -2133,18 +2192,18 @@
         <v>10000</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I26:I31" si="5">F26*1.125</f>
+        <f t="shared" ref="I26:I31" si="6">F26*1.125</f>
         <v>22500</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J31" si="6">I26/D26</f>
+        <f t="shared" ref="J26:J31" si="7">I26/D26</f>
         <v>22500</v>
       </c>
       <c r="K26">
@@ -2168,7 +2227,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="str">
-        <f>CONCATENATE("V-",B27,"-",D27,"-",E27,"-",G27,"-",K27,"-",L27,"-",P27)</f>
+        <f t="shared" si="0"/>
         <v>V-26-2-10000-2-10-GS-</v>
       </c>
       <c r="D27">
@@ -2178,18 +2237,18 @@
         <v>10000</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
       <c r="I27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22500</v>
       </c>
       <c r="J27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11250</v>
       </c>
       <c r="K27">
@@ -2213,7 +2272,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="str">
-        <f>CONCATENATE("V-",B28,"-",D28,"-",E28,"-",G28,"-",K28,"-",L28,"-",P28)</f>
+        <f t="shared" si="0"/>
         <v>V-27-5-10000-2-10-GS-</v>
       </c>
       <c r="D28">
@@ -2223,18 +2282,18 @@
         <v>10000</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="G28">
         <v>2</v>
       </c>
       <c r="I28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22500</v>
       </c>
       <c r="J28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4500</v>
       </c>
       <c r="K28">
@@ -2258,7 +2317,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="str">
-        <f>CONCATENATE("V-",B29,"-",D29,"-",E29,"-",G29,"-",K29,"-",L29,"-",P29)</f>
+        <f t="shared" si="0"/>
         <v>V-28-10-10000-2-10-GS-</v>
       </c>
       <c r="D29">
@@ -2268,18 +2327,18 @@
         <v>10000</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="G29">
         <v>2</v>
       </c>
       <c r="I29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22500</v>
       </c>
       <c r="J29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2250</v>
       </c>
       <c r="K29">
@@ -2303,7 +2362,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="str">
-        <f>CONCATENATE("V-",B30,"-",D30,"-",E30,"-",G30,"-",K30,"-",L30,"-",P30)</f>
+        <f t="shared" si="0"/>
         <v>V-29-25-10000-2-10-GS-</v>
       </c>
       <c r="D30">
@@ -2313,18 +2372,18 @@
         <v>10000</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="I30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22500</v>
       </c>
       <c r="J30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>900</v>
       </c>
       <c r="K30">
@@ -2348,7 +2407,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="str">
-        <f>CONCATENATE("V-",B31,"-",D31,"-",E31,"-",G31,"-",K31,"-",L31,"-",P31)</f>
+        <f t="shared" si="0"/>
         <v>V-30-50-10000-2-10-GS-</v>
       </c>
       <c r="D31">
@@ -2358,18 +2417,18 @@
         <v>10000</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20000</v>
       </c>
       <c r="G31">
         <v>2</v>
       </c>
       <c r="I31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22500</v>
       </c>
       <c r="J31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>450</v>
       </c>
       <c r="K31">
@@ -2396,6 +2455,154 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C14F885-A944-4AA3-A80A-D81424F5B467}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9">
+        <f>B2*B3*B4*B5*B6*B7*B8</f>
+        <v>51840</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E22C6B-9931-41BB-9D7A-4E68C86B3DDF}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B737E7BE-69D6-45B4-A8E9-BE91942F4A81}">
   <dimension ref="A1:M1010"/>
   <sheetViews>
@@ -33729,7 +33936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D272F9-C60B-4199-8657-134ADD5033E3}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -33867,7 +34074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77CCE48-7B7D-463E-97D6-7C4A5240B20A}">
   <dimension ref="A1:R17"/>
   <sheetViews>
@@ -34046,7 +34253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4854F1-8777-479C-BD9C-DA49037684CB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -34058,7 +34265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0258F8-66E4-458F-9496-1395E830828D}">
   <dimension ref="A2:I30"/>
   <sheetViews>

</xml_diff>